<commit_message>
modificacion en el estudio
</commit_message>
<xml_diff>
--- a/documentos/modelos finales/Modelos Datos fijos modificacion.xlsx
+++ b/documentos/modelos finales/Modelos Datos fijos modificacion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\datos\Mis documentos\GitHub\LibroSueldoDigital\documentos\modelos finales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JAVIER\Documents\GitHub\LibroSueldoDigital\documentos\modelos finales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7B14412-B87D-4719-A087-95EFFE491312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2A26FD5-199E-4C2A-9271-65B34F1B7C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{5E66E99B-3367-44EE-9783-6944D3DEB6D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5E66E99B-3367-44EE-9783-6944D3DEB6D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
   <si>
     <t>LIBRO DE SUELDOS DIGITAL - AFIP</t>
   </si>
@@ -262,7 +262,13 @@
     <t>PEDROZO DANTE OSCALDO</t>
   </si>
   <si>
-    <t>art17 trab temp</t>
+    <t>BRIZUELA JUAN ANDRES RAMON</t>
+  </si>
+  <si>
+    <t>NAVARRO JANATAN FACUNDO</t>
+  </si>
+  <si>
+    <t>PEON GRAL</t>
   </si>
 </sst>
 </file>
@@ -895,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83205A9D-0CEA-4714-8546-E299B9B69775}">
   <dimension ref="A1:AL21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,7 +1371,7 @@
         <v>31</v>
       </c>
       <c r="F7" s="30" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G7" s="30"/>
       <c r="H7" s="30">
@@ -1375,7 +1381,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" s="30">
         <v>0</v>
@@ -1462,83 +1468,227 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B8" s="19"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="30"/>
+    <row r="8" spans="1:38" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="22">
+        <v>20412270089</v>
+      </c>
+      <c r="D8" s="28">
+        <v>30</v>
+      </c>
+      <c r="E8" s="29">
+        <v>32</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>71</v>
+      </c>
       <c r="G8" s="32"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="30"/>
-      <c r="N8" s="30"/>
-      <c r="O8" s="30"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="32"/>
-      <c r="S8" s="30"/>
-      <c r="T8" s="30"/>
-      <c r="U8" s="30"/>
-      <c r="V8" s="30"/>
-      <c r="W8" s="30"/>
-      <c r="X8" s="30"/>
-      <c r="Y8" s="30"/>
-      <c r="Z8" s="30"/>
-      <c r="AA8" s="30"/>
-      <c r="AB8" s="30"/>
-      <c r="AC8" s="30"/>
-      <c r="AD8" s="30"/>
-      <c r="AE8" s="30"/>
-      <c r="AF8" s="31"/>
-      <c r="AG8" s="31"/>
-      <c r="AH8" s="31"/>
-      <c r="AI8" s="31"/>
-      <c r="AJ8" s="31"/>
-      <c r="AK8" s="31"/>
-      <c r="AL8" s="31"/>
+      <c r="H8" s="30">
+        <v>30</v>
+      </c>
+      <c r="I8" s="30">
+        <v>1</v>
+      </c>
+      <c r="J8" s="30">
+        <v>0</v>
+      </c>
+      <c r="K8" s="30">
+        <v>0</v>
+      </c>
+      <c r="L8" s="30">
+        <v>0</v>
+      </c>
+      <c r="M8" s="30">
+        <v>0</v>
+      </c>
+      <c r="N8" s="30">
+        <v>1</v>
+      </c>
+      <c r="O8" s="30">
+        <v>1</v>
+      </c>
+      <c r="P8" s="30">
+        <v>5</v>
+      </c>
+      <c r="Q8" s="30">
+        <v>97</v>
+      </c>
+      <c r="R8" s="32">
+        <v>111</v>
+      </c>
+      <c r="S8" s="30">
+        <v>0</v>
+      </c>
+      <c r="T8" s="30">
+        <v>27</v>
+      </c>
+      <c r="U8" s="30">
+        <v>1</v>
+      </c>
+      <c r="V8" s="30">
+        <v>1</v>
+      </c>
+      <c r="W8" s="30">
+        <v>0</v>
+      </c>
+      <c r="X8" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="30">
+        <v>30</v>
+      </c>
+      <c r="AB8" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="30">
+        <v>2</v>
+      </c>
+      <c r="AE8" s="30">
+        <v>119302</v>
+      </c>
+      <c r="AF8" s="31">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="31">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="31">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="31">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="31">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="B9" s="19"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="30"/>
+    <row r="9" spans="1:38" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="22">
+        <v>20363899952</v>
+      </c>
+      <c r="D9" s="28">
+        <v>30</v>
+      </c>
+      <c r="E9" s="29">
+        <v>51</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>71</v>
+      </c>
       <c r="G9" s="32"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="32"/>
-      <c r="S9" s="30"/>
-      <c r="T9" s="30"/>
-      <c r="U9" s="30"/>
-      <c r="V9" s="30"/>
-      <c r="W9" s="30"/>
-      <c r="X9" s="30"/>
-      <c r="Y9" s="30"/>
-      <c r="Z9" s="30"/>
-      <c r="AA9" s="30"/>
-      <c r="AB9" s="30"/>
-      <c r="AC9" s="30"/>
-      <c r="AD9" s="30"/>
-      <c r="AE9" s="30"/>
-      <c r="AF9" s="31"/>
-      <c r="AG9" s="31"/>
-      <c r="AH9" s="31"/>
-      <c r="AI9" s="31"/>
-      <c r="AJ9" s="31"/>
-      <c r="AK9" s="31"/>
-      <c r="AL9" s="31"/>
+      <c r="H9" s="30">
+        <v>30</v>
+      </c>
+      <c r="I9" s="30">
+        <v>1</v>
+      </c>
+      <c r="J9" s="30">
+        <v>0</v>
+      </c>
+      <c r="K9" s="30">
+        <v>0</v>
+      </c>
+      <c r="L9" s="30">
+        <v>0</v>
+      </c>
+      <c r="M9" s="30">
+        <v>0</v>
+      </c>
+      <c r="N9" s="30">
+        <v>1</v>
+      </c>
+      <c r="O9" s="30">
+        <v>1</v>
+      </c>
+      <c r="P9" s="30">
+        <v>5</v>
+      </c>
+      <c r="Q9" s="30">
+        <v>97</v>
+      </c>
+      <c r="R9" s="32">
+        <v>111</v>
+      </c>
+      <c r="S9" s="30">
+        <v>0</v>
+      </c>
+      <c r="T9" s="30">
+        <v>27</v>
+      </c>
+      <c r="U9" s="30">
+        <v>1</v>
+      </c>
+      <c r="V9" s="30">
+        <v>1</v>
+      </c>
+      <c r="W9" s="30">
+        <v>0</v>
+      </c>
+      <c r="X9" s="30">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="30">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="30">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="30">
+        <v>30</v>
+      </c>
+      <c r="AB9" s="30">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="30">
+        <v>2</v>
+      </c>
+      <c r="AE9" s="30">
+        <v>119302</v>
+      </c>
+      <c r="AF9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="31">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B10" s="19"/>
@@ -1569,15 +1719,33 @@
       <c r="AA10" s="30"/>
       <c r="AB10" s="30"/>
       <c r="AC10" s="30"/>
-      <c r="AD10" s="30"/>
-      <c r="AE10" s="30"/>
-      <c r="AF10" s="31"/>
-      <c r="AG10" s="31"/>
-      <c r="AH10" s="31"/>
-      <c r="AI10" s="31"/>
-      <c r="AJ10" s="31"/>
-      <c r="AK10" s="31"/>
-      <c r="AL10" s="31"/>
+      <c r="AD10" s="30">
+        <v>2</v>
+      </c>
+      <c r="AE10" s="30">
+        <v>119302</v>
+      </c>
+      <c r="AF10" s="31">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="31">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="31">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="31">
+        <v>0</v>
+      </c>
+      <c r="AL10" s="31">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B11" s="19"/>
@@ -1608,15 +1776,33 @@
       <c r="AA11" s="30"/>
       <c r="AB11" s="30"/>
       <c r="AC11" s="30"/>
-      <c r="AD11" s="30"/>
-      <c r="AE11" s="30"/>
-      <c r="AF11" s="31"/>
-      <c r="AG11" s="31"/>
-      <c r="AH11" s="31"/>
-      <c r="AI11" s="31"/>
-      <c r="AJ11" s="31"/>
-      <c r="AK11" s="31"/>
-      <c r="AL11" s="31"/>
+      <c r="AD11" s="30">
+        <v>2</v>
+      </c>
+      <c r="AE11" s="30">
+        <v>119302</v>
+      </c>
+      <c r="AF11" s="31">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="31">
+        <v>0</v>
+      </c>
+      <c r="AH11" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="31">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="31">
+        <v>0</v>
+      </c>
+      <c r="AL11" s="31">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B12" s="19"/>
@@ -1647,15 +1833,33 @@
       <c r="AA12" s="30"/>
       <c r="AB12" s="30"/>
       <c r="AC12" s="30"/>
-      <c r="AD12" s="30"/>
-      <c r="AE12" s="30"/>
-      <c r="AF12" s="31"/>
-      <c r="AG12" s="31"/>
-      <c r="AH12" s="31"/>
-      <c r="AI12" s="31"/>
-      <c r="AJ12" s="31"/>
-      <c r="AK12" s="31"/>
-      <c r="AL12" s="31"/>
+      <c r="AD12" s="30">
+        <v>2</v>
+      </c>
+      <c r="AE12" s="30">
+        <v>119302</v>
+      </c>
+      <c r="AF12" s="31">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="31">
+        <v>0</v>
+      </c>
+      <c r="AH12" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI12" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="31">
+        <v>0</v>
+      </c>
+      <c r="AK12" s="31">
+        <v>0</v>
+      </c>
+      <c r="AL12" s="31">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B13" s="20"/>
@@ -1686,15 +1890,33 @@
       <c r="AA13" s="30"/>
       <c r="AB13" s="30"/>
       <c r="AC13" s="30"/>
-      <c r="AD13" s="30"/>
-      <c r="AE13" s="30"/>
-      <c r="AF13" s="31"/>
-      <c r="AG13" s="31"/>
-      <c r="AH13" s="31"/>
-      <c r="AI13" s="31"/>
-      <c r="AJ13" s="31"/>
-      <c r="AK13" s="31"/>
-      <c r="AL13" s="31"/>
+      <c r="AD13" s="30">
+        <v>2</v>
+      </c>
+      <c r="AE13" s="30">
+        <v>119302</v>
+      </c>
+      <c r="AF13" s="31">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="31">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="31">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="31">
+        <v>0</v>
+      </c>
+      <c r="AL13" s="31">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B14" s="19"/>
@@ -1725,15 +1947,33 @@
       <c r="AA14" s="30"/>
       <c r="AB14" s="30"/>
       <c r="AC14" s="30"/>
-      <c r="AD14" s="30"/>
-      <c r="AE14" s="30"/>
-      <c r="AF14" s="31"/>
-      <c r="AG14" s="31"/>
-      <c r="AH14" s="31"/>
-      <c r="AI14" s="31"/>
-      <c r="AJ14" s="31"/>
-      <c r="AK14" s="31"/>
-      <c r="AL14" s="31"/>
+      <c r="AD14" s="30">
+        <v>2</v>
+      </c>
+      <c r="AE14" s="30">
+        <v>119302</v>
+      </c>
+      <c r="AF14" s="31">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="31">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="31">
+        <v>0</v>
+      </c>
+      <c r="AK14" s="31">
+        <v>0</v>
+      </c>
+      <c r="AL14" s="31">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B15" s="19"/>
@@ -1764,15 +2004,33 @@
       <c r="AA15" s="30"/>
       <c r="AB15" s="30"/>
       <c r="AC15" s="30"/>
-      <c r="AD15" s="30"/>
-      <c r="AE15" s="30"/>
-      <c r="AF15" s="31"/>
-      <c r="AG15" s="31"/>
-      <c r="AH15" s="31"/>
-      <c r="AI15" s="31"/>
-      <c r="AJ15" s="31"/>
-      <c r="AK15" s="31"/>
-      <c r="AL15" s="31"/>
+      <c r="AD15" s="30">
+        <v>2</v>
+      </c>
+      <c r="AE15" s="30">
+        <v>119302</v>
+      </c>
+      <c r="AF15" s="31">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="31">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="31">
+        <v>0</v>
+      </c>
+      <c r="AK15" s="31">
+        <v>0</v>
+      </c>
+      <c r="AL15" s="31">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B16" s="19"/>
@@ -1803,15 +2061,33 @@
       <c r="AA16" s="30"/>
       <c r="AB16" s="30"/>
       <c r="AC16" s="30"/>
-      <c r="AD16" s="30"/>
-      <c r="AE16" s="30"/>
-      <c r="AF16" s="31"/>
-      <c r="AG16" s="31"/>
-      <c r="AH16" s="31"/>
-      <c r="AI16" s="31"/>
-      <c r="AJ16" s="31"/>
-      <c r="AK16" s="31"/>
-      <c r="AL16" s="31"/>
+      <c r="AD16" s="30">
+        <v>2</v>
+      </c>
+      <c r="AE16" s="30">
+        <v>119302</v>
+      </c>
+      <c r="AF16" s="31">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="31">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="31">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="31">
+        <v>0</v>
+      </c>
+      <c r="AL16" s="31">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B17" s="19"/>
@@ -1842,15 +2118,33 @@
       <c r="AA17" s="30"/>
       <c r="AB17" s="30"/>
       <c r="AC17" s="30"/>
-      <c r="AD17" s="30"/>
-      <c r="AE17" s="30"/>
-      <c r="AF17" s="31"/>
-      <c r="AG17" s="31"/>
-      <c r="AH17" s="31"/>
-      <c r="AI17" s="31"/>
-      <c r="AJ17" s="31"/>
-      <c r="AK17" s="31"/>
-      <c r="AL17" s="31"/>
+      <c r="AD17" s="30">
+        <v>2</v>
+      </c>
+      <c r="AE17" s="30">
+        <v>119302</v>
+      </c>
+      <c r="AF17" s="31">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="31">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI17" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="31">
+        <v>0</v>
+      </c>
+      <c r="AK17" s="31">
+        <v>0</v>
+      </c>
+      <c r="AL17" s="31">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B18" s="19"/>
@@ -1881,15 +2175,33 @@
       <c r="AA18" s="30"/>
       <c r="AB18" s="30"/>
       <c r="AC18" s="30"/>
-      <c r="AD18" s="30"/>
-      <c r="AE18" s="30"/>
-      <c r="AF18" s="31"/>
-      <c r="AG18" s="31"/>
-      <c r="AH18" s="31"/>
-      <c r="AI18" s="31"/>
-      <c r="AJ18" s="31"/>
-      <c r="AK18" s="31"/>
-      <c r="AL18" s="31"/>
+      <c r="AD18" s="30">
+        <v>2</v>
+      </c>
+      <c r="AE18" s="30">
+        <v>119302</v>
+      </c>
+      <c r="AF18" s="31">
+        <v>0</v>
+      </c>
+      <c r="AG18" s="31">
+        <v>0</v>
+      </c>
+      <c r="AH18" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI18" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="31">
+        <v>0</v>
+      </c>
+      <c r="AK18" s="31">
+        <v>0</v>
+      </c>
+      <c r="AL18" s="31">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B19" s="19"/>
@@ -1920,15 +2232,33 @@
       <c r="AA19" s="30"/>
       <c r="AB19" s="30"/>
       <c r="AC19" s="30"/>
-      <c r="AD19" s="30"/>
-      <c r="AE19" s="30"/>
-      <c r="AF19" s="31"/>
-      <c r="AG19" s="31"/>
-      <c r="AH19" s="31"/>
-      <c r="AI19" s="31"/>
-      <c r="AJ19" s="31"/>
-      <c r="AK19" s="31"/>
-      <c r="AL19" s="31"/>
+      <c r="AD19" s="30">
+        <v>2</v>
+      </c>
+      <c r="AE19" s="30">
+        <v>119302</v>
+      </c>
+      <c r="AF19" s="31">
+        <v>0</v>
+      </c>
+      <c r="AG19" s="31">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI19" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ19" s="31">
+        <v>0</v>
+      </c>
+      <c r="AK19" s="31">
+        <v>0</v>
+      </c>
+      <c r="AL19" s="31">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="2:38" x14ac:dyDescent="0.25">
       <c r="L20" s="18"/>

</xml_diff>